<commit_message>
chore: Replaced CR1220 battery with super capacitor
</commit_message>
<xml_diff>
--- a/hardware/bom4china.xlsx
+++ b/hardware/bom4china.xlsx
@@ -58,30 +58,33 @@
     <t xml:space="preserve">BT1</t>
   </si>
   <si>
-    <t xml:space="preserve">BAT+3V</t>
+    <t xml:space="preserve">DMS3R3</t>
   </si>
   <si>
     <t xml:space="preserve">~</t>
   </si>
   <si>
-    <t xml:space="preserve">Battery:BatteryHolder_LINX_BAT-HLD-012-SMT</t>
+    <t xml:space="preserve">Battery:BatteryHolder_Seiko_MS621F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淘宝</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMS3R3224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1,C2,C9,C10,C11,C17,C18,C20,C21,C23,C25,C26,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C45,C55,C56,C57,C58,C59,C64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
   </si>
   <si>
     <t xml:space="preserve">立创商城</t>
   </si>
   <si>
-    <t xml:space="preserve">C964817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1,C2,C9,C10,C11,C17,C18,C20,C21,C23,C25,C26,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C45,C55,C56,C57,C58,C59,C64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">C701321</t>
   </si>
   <si>
@@ -221,9 +224,6 @@
   </si>
   <si>
     <t xml:space="preserve">TerminalBlock:TerminalBlock_bornier-2_P5.08mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">淘宝</t>
   </si>
   <si>
     <t xml:space="preserve">KF301-2P</t>
@@ -926,7 +926,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK TC"/>
@@ -953,6 +953,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -997,7 +1002,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1015,6 +1020,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1045,8 +1054,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J66" activeCellId="0" sqref="J66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1101,25 +1110,25 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -1138,64 +1147,64 @@
         <v>29</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>6</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -1207,41 +1216,41 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
@@ -1253,18 +1262,18 @@
         <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>12</v>
@@ -1276,18 +1285,18 @@
         <v>4</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>12</v>
@@ -1299,18 +1308,18 @@
         <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
@@ -1322,122 +1331,122 @@
         <v>6</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>44</v>
+        <v>19</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="115" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>7</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="4" t="s">
@@ -1461,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>71</v>
@@ -1478,13 +1487,13 @@
         <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>74</v>
@@ -1507,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>78</v>
@@ -1530,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>71</v>
@@ -1553,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>71</v>
@@ -1576,7 +1585,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>87</v>
@@ -1599,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>91</v>
@@ -1622,7 +1631,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>95</v>
@@ -1645,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>95</v>
@@ -1668,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>95</v>
@@ -1685,13 +1694,13 @@
         <v>12</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>74</v>
@@ -1708,13 +1717,13 @@
         <v>12</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>74</v>
@@ -1731,13 +1740,13 @@
         <v>12</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>74</v>
@@ -1760,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>109</v>
@@ -1783,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>109</v>
@@ -1806,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>109</v>
@@ -1829,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>117</v>
@@ -1853,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>121</v>
@@ -1877,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>125</v>
@@ -1901,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>127</v>
@@ -1925,7 +1934,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>130</v>
@@ -1948,7 +1957,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>133</v>
@@ -1971,7 +1980,7 @@
         <v>13</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>136</v>
@@ -1994,7 +2003,7 @@
         <v>15</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>138</v>
@@ -2017,7 +2026,7 @@
         <v>8</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>141</v>
@@ -2040,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>143</v>
@@ -2063,7 +2072,7 @@
         <v>6</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>146</v>
@@ -2086,9 +2095,9 @@
         <v>3</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2109,9 +2118,9 @@
         <v>6</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2132,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>133</v>
@@ -2155,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>158</v>
@@ -2178,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>162</v>
@@ -2201,7 +2210,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>166</v>
@@ -2224,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>170</v>
@@ -2247,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>166</v>
@@ -2475,7 +2484,7 @@
         <v>2</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>203</v>
@@ -2521,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H64" s="0"/>
       <c r="I64" s="4" t="s">
@@ -2545,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H65" s="0"/>
       <c r="I65" s="3" t="s">
@@ -2569,7 +2578,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H66" s="0"/>
       <c r="I66" s="4" t="s">
@@ -2596,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H67" s="0"/>
       <c r="I67" s="4" t="s">
@@ -2623,7 +2632,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H68" s="0"/>
       <c r="I68" s="3" t="s">
@@ -2647,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H69" s="0"/>
       <c r="I69" s="3" t="s">
@@ -2674,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H70" s="0"/>
       <c r="I70" s="3" t="s">
@@ -2701,7 +2710,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H71" s="0"/>
       <c r="I71" s="3" t="s">
@@ -2728,7 +2737,7 @@
         <v>3</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H72" s="0"/>
       <c r="I72" s="3" t="s">
@@ -2755,7 +2764,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H73" s="0"/>
       <c r="I73" s="3" t="s">
@@ -2779,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H74" s="0"/>
       <c r="I74" s="4" t="s">
@@ -2803,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H75" s="0"/>
       <c r="I75" s="3" t="s">

</xml_diff>

<commit_message>
docs: Update remarks on STM32F103, MAX3232
</commit_message>
<xml_diff>
--- a/hardware/bom4china.xlsx
+++ b/hardware/bom4china.xlsx
@@ -776,7 +776,7 @@
     <t xml:space="preserve">MAX3485 SOIC</t>
   </si>
   <si>
-    <t xml:space="preserve">SP3485 也可</t>
+    <t xml:space="preserve">SP3485、MAX13487 等均可</t>
   </si>
   <si>
     <t xml:space="preserve">U10</t>
@@ -810,7 +810,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">、</t>
+      <t xml:space="preserve">（已测试通过）、</t>
     </r>
     <r>
       <rPr>
@@ -846,7 +846,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">等均可替代</t>
+      <t xml:space="preserve">等均可替代，但注意可能存在兼容性问题，需要修改代码</t>
     </r>
   </si>
   <si>
@@ -865,7 +865,7 @@
     <t xml:space="preserve">MAX3232 SOIC</t>
   </si>
   <si>
-    <t xml:space="preserve">SP3232 也可</t>
+    <t xml:space="preserve">MAX3232 假货极多，留意价格，或可用 SP3232 等代换</t>
   </si>
   <si>
     <t xml:space="preserve">U12,U13,U14</t>
@@ -926,7 +926,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK TC"/>
@@ -953,11 +953,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1002,7 +997,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1020,10 +1015,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1054,8 +1045,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B66" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J71" activeCellId="0" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1110,13 +1101,13 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -1333,7 +1324,7 @@
       <c r="G11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2097,7 +2088,7 @@
       <c r="G44" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="H44" s="5" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2120,7 +2111,7 @@
       <c r="G45" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" s="5" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2513,7 +2504,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
         <v>205</v>
       </c>
@@ -2666,7 +2657,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="58.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
         <v>237</v>
       </c>

</xml_diff>